<commit_message>
Update inputs and outputs
</commit_message>
<xml_diff>
--- a/sample_inputs/Success_Story_Export.xlsx
+++ b/sample_inputs/Success_Story_Export.xlsx
@@ -514,7 +514,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nightly Export User (Don't Edit!) on 06/21/2022 at 03:07:21 AM</t>
+          <t>Nightly Export User (Don't Edit!) on 06/28/2022 at 03:07:13 AM</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BE219"/>
+  <dimension ref="A1:BE226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1361,7 +1361,7 @@
     <col width="75.7109375" customWidth="1" min="10" max="10"/>
     <col width="42.7109375" customWidth="1" min="11" max="11"/>
     <col width="8.7109375" customWidth="1" min="12" max="12"/>
-    <col width="63.7109375" customWidth="1" min="13" max="13"/>
+    <col width="58.7109375" customWidth="1" min="13" max="13"/>
     <col width="20.7109375" customWidth="1" min="14" max="14"/>
     <col width="75.7109375" customWidth="1" min="15" max="15"/>
     <col width="25.7109375" customWidth="1" min="16" max="16"/>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Dustin Fritsche</t>
+          <t>User 14706</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Ana Lemke</t>
+          <t>User 14409</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Patsy Bishop</t>
+          <t>User 14365</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -2317,7 +2317,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Patsy Bishop</t>
+          <t>User 14365</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Mary Napolitano</t>
+          <t>User 14346</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Barbara Curry</t>
+          <t>User 14366</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -2915,7 +2915,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Sheila Miller</t>
+          <t>User 17677</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -3112,7 +3112,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Jenna Smith</t>
+          <t>User 14547</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Beth Dellatori</t>
+          <t>User 20288</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -3702,7 +3702,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Aruna Budhram</t>
+          <t>User 15626</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Duane Friend</t>
+          <t>User 14507</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Cheri Burcham</t>
+          <t>User 14515</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -4243,7 +4243,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Mary Fischer</t>
+          <t>User 20317</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -4410,7 +4410,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Erin Garrett</t>
+          <t>User 16098</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -4574,12 +4574,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Erin Garrett</t>
+          <t>User 16098</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>User 14271, Stanley (Jay) Solomon, User 14507, User 14508, User 15637, User 16098, User 16782, User 17879, User 18147, User 20616</t>
+          <t>User 14271, User 14505, User 14507, User 14508, User 15637, User 16098, User 16782, User 17879, User 18147, User 20616</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -4741,7 +4741,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Talon Becker</t>
+          <t>User 14485</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -4917,7 +4917,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Robin Johnston</t>
+          <t>User 14798</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -5124,7 +5124,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Elizabeth Wahle</t>
+          <t>User 14528</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Brittnay Haag</t>
+          <t>User 14714</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -5515,7 +5515,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Carrie Eldridge</t>
+          <t>User 21133</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -5720,7 +5720,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Carrie McKillip</t>
+          <t>User 14487</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -5916,7 +5916,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -6076,7 +6076,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -6231,7 +6231,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Erin Garrett</t>
+          <t>User 16098</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -6404,7 +6404,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Emily Schoenfelder</t>
+          <t>User 14455</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -6583,7 +6583,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Nick Brown</t>
+          <t>User 20907</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -6780,7 +6780,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Leilah Siegel</t>
+          <t>User 21199</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -6942,7 +6942,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Misty Bernhard</t>
+          <t>User 20909</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -7142,7 +7142,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Grace Margherio</t>
+          <t>User 19977</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -7346,7 +7346,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Douglas B. Gucker</t>
+          <t>User 14537</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -7509,7 +7509,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Stanley (Jay) Solomon</t>
+          <t>User 14505</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -7519,12 +7519,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Stanley (Jay) Solomon</t>
+          <t>User 14505</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Stanley (Jay) Solomon, User 17891</t>
+          <t>User 14505, User 17891</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Julie Dantone</t>
+          <t>User 18475</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -7893,7 +7893,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
@@ -8097,7 +8097,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -8301,7 +8301,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -8505,7 +8505,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -8709,7 +8709,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -8913,7 +8913,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -9117,7 +9117,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -9321,7 +9321,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -9525,7 +9525,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Rachel Hazen</t>
+          <t>User 15144</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -9723,7 +9723,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Carol VanMatre</t>
+          <t>User 14416</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -9927,7 +9927,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Grant McCarty</t>
+          <t>User 14535</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -10108,7 +10108,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Sarah Vogel</t>
+          <t>User 19879</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -10318,7 +10318,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Jennifer Fishburn</t>
+          <t>User 14525</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -10514,7 +10514,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Michelle Cox</t>
+          <t>User 14467</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -10702,7 +10702,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Sarah Farley</t>
+          <t>User 20187</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -10872,7 +10872,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Emily Swihart</t>
+          <t>User 21721</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -11042,7 +11042,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Phillip Alberti</t>
+          <t>User 16485</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -11215,7 +11215,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Bruce Black</t>
+          <t>User 14530</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -11233,7 +11233,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>First Presbyterian Church - Dixon, IL (Dixon Community Gardens)</t>
+          <t>First Presbyterian Church - Dixon Community Gardens</t>
         </is>
       </c>
       <c r="N52" t="n">
@@ -11251,7 +11251,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>110 E 3rd St.</t>
+          <t>110 E 3rd St</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -11425,7 +11425,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>Emily Swihart</t>
+          <t>User 21721</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -11595,7 +11595,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Bruce Black</t>
+          <t>User 14530</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -11787,7 +11787,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Martha Ebbesmeyer</t>
+          <t>User 14451</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -11949,7 +11949,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Carissa Davis</t>
+          <t>User 14459</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -12118,7 +12118,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Meghan McCleary</t>
+          <t>User 14573</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -12280,7 +12280,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>Durriyyah Kemp</t>
+          <t>User 14500</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -12494,7 +12494,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Kathryn Pereira</t>
+          <t>User 18977</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -12672,7 +12672,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>Erin Maxwell</t>
+          <t>User 14405</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -12867,7 +12867,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Zachary Grant</t>
+          <t>User 14543</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -13049,7 +13049,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Peggy Doty</t>
+          <t>User 14508</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -13272,7 +13272,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -13467,7 +13467,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Nathan Johanning</t>
+          <t>User 14542</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -13667,7 +13667,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>Katharine Parker</t>
+          <t>User 19190</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
@@ -13864,7 +13864,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>Erin Harper</t>
+          <t>User 19293</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -14066,7 +14066,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -14261,7 +14261,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>Abigail Garofalo</t>
+          <t>User 17879</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -14452,7 +14452,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -14647,7 +14647,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>Michael Delany</t>
+          <t>User 20349</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
@@ -15006,7 +15006,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>Nicole Flowers-Kimmerle</t>
+          <t>User 18705</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -15215,7 +15215,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>Christopher Enroth</t>
+          <t>User 14520</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -15386,7 +15386,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>Sandra Prez</t>
+          <t>User 14476</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -15592,7 +15592,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>Andrew Holsinger</t>
+          <t>User 14527</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -15771,7 +15771,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>Christopher Enroth</t>
+          <t>User 14520</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -15933,7 +15933,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>Sonia Lopez</t>
+          <t>User 14501</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
@@ -16115,7 +16115,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>Nancy Kreith</t>
+          <t>User 14533</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
@@ -16327,7 +16327,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Stanley (Jay) Solomon</t>
+          <t>User 14505</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -16337,12 +16337,12 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>Stanley (Jay) Solomon</t>
+          <t>User 14505</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Stanley (Jay) Solomon, User 17891</t>
+          <t>User 14505, User 17891</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -16512,7 +16512,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>Tiffany Macke</t>
+          <t>User 14491</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -16674,7 +16674,7 @@
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>Elizabeth Hartke</t>
+          <t>User 15233</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
@@ -16874,7 +16874,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>Tiffney Stewart</t>
+          <t>User 14364</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -17071,7 +17071,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>Barbara Curry</t>
+          <t>User 14366</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
@@ -17275,7 +17275,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>Rachel Benn</t>
+          <t>User 15793</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
@@ -17420,7 +17420,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>Christina Lueking</t>
+          <t>User 14703</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
@@ -17627,7 +17627,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>Carrie Eldridge</t>
+          <t>User 21133</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -17832,7 +17832,7 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>Ana Lemke</t>
+          <t>User 14409</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
@@ -18026,7 +18026,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>MaryBeth Massey</t>
+          <t>User 14400</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
@@ -18239,7 +18239,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>Miguel Palacios Hidalgo</t>
+          <t>User 15777</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
@@ -18443,7 +18443,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>Miguel Palacios Hidalgo</t>
+          <t>User 15777</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
@@ -18648,7 +18648,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>Rima Abusaid</t>
+          <t>User 16603</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -18863,7 +18863,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>Rima Abusaid</t>
+          <t>User 16603</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
@@ -19075,7 +19075,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>Sarita Sawyer</t>
+          <t>User 14363</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -19276,7 +19276,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>Sarita Sawyer</t>
+          <t>User 14363</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -19476,7 +19476,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>Wren Woodburn</t>
+          <t>User 20382</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -19675,7 +19675,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>Afiwa Tete</t>
+          <t>User 14687</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -19868,7 +19868,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>Tonya Fitzpatrick</t>
+          <t>User 21078</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -20063,7 +20063,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>Tonya Fitzpatrick</t>
+          <t>User 21078</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -20258,7 +20258,7 @@
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>Laura Holland</t>
+          <t>User 14683</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -20461,7 +20461,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>Russell  Medley</t>
+          <t>User 14496</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -20692,7 +20692,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>Katherine Ellis</t>
+          <t>User 14795</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
@@ -20887,7 +20887,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>Elizabeth Repplinger</t>
+          <t>User 14688</t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
@@ -21084,7 +21084,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>Tonya Fitzpatrick</t>
+          <t>User 21078</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
@@ -21279,7 +21279,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>Barbara Curry</t>
+          <t>User 14366</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
@@ -21483,7 +21483,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
@@ -21691,7 +21691,7 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>Ana Lemke</t>
+          <t>User 14409</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
@@ -21857,7 +21857,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>Sara Attig</t>
+          <t>User 14677</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
@@ -22062,7 +22062,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>Shirley Vouris</t>
+          <t>User 14862</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
@@ -22284,7 +22284,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>Shirley Vouris</t>
+          <t>User 14862</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
@@ -22510,7 +22510,7 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>Shirley Vouris</t>
+          <t>User 14862</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
@@ -22723,7 +22723,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
@@ -22878,7 +22878,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J112" t="inlineStr">
@@ -23033,7 +23033,7 @@
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>Julie Tyberendt Fulton</t>
+          <t>User 14408</t>
         </is>
       </c>
       <c r="J113" t="inlineStr">
@@ -23233,7 +23233,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>Carol Erickson</t>
+          <t>User 14758</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
@@ -23460,7 +23460,7 @@
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>Carol Erickson</t>
+          <t>User 14758</t>
         </is>
       </c>
       <c r="J115" t="inlineStr">
@@ -23676,7 +23676,7 @@
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>Carol Erickson</t>
+          <t>User 14758</t>
         </is>
       </c>
       <c r="J116" t="inlineStr">
@@ -23892,7 +23892,7 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>Pam Schallhorn</t>
+          <t>User 14290</t>
         </is>
       </c>
       <c r="J117" t="inlineStr">
@@ -24114,7 +24114,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>Beth Kraft</t>
+          <t>User 14380</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
@@ -24316,7 +24316,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>Beth Kraft</t>
+          <t>User 14380</t>
         </is>
       </c>
       <c r="J119" t="inlineStr">
@@ -24513,7 +24513,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>Hope Dennis</t>
+          <t>User 14404</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -24713,7 +24713,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>Hope Dennis</t>
+          <t>User 14404</t>
         </is>
       </c>
       <c r="J121" t="inlineStr">
@@ -24913,7 +24913,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J122" t="inlineStr">
@@ -25127,7 +25127,7 @@
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>Jo Stine</t>
+          <t>User 14406</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -25323,7 +25323,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>Brooke Desper</t>
+          <t>User 21080</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -25522,7 +25522,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>Julie Dantone</t>
+          <t>User 18475</t>
         </is>
       </c>
       <c r="J125" t="inlineStr">
@@ -25711,7 +25711,7 @@
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>Julie Dantone</t>
+          <t>User 18475</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
@@ -25900,7 +25900,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>Julie Dantone</t>
+          <t>User 18475</t>
         </is>
       </c>
       <c r="J127" t="inlineStr">
@@ -26091,7 +26091,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>Julie Tyberendt Fulton</t>
+          <t>User 14408</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
@@ -26291,7 +26291,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>Ana Lemke</t>
+          <t>User 14409</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
@@ -26485,7 +26485,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>Erin Maxwell</t>
+          <t>User 14405</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
@@ -26680,7 +26680,7 @@
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J131" t="inlineStr">
@@ -26875,7 +26875,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J132" t="inlineStr">
@@ -27070,7 +27070,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>Barbara Curry</t>
+          <t>User 14366</t>
         </is>
       </c>
       <c r="J133" t="inlineStr">
@@ -27274,7 +27274,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>Joey Fonseca</t>
+          <t>User 20553</t>
         </is>
       </c>
       <c r="J134" t="inlineStr">
@@ -27491,7 +27491,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>Marcia Cruse</t>
+          <t>User 15185</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
@@ -27694,7 +27694,7 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>Dale Kehr</t>
+          <t>User 14566</t>
         </is>
       </c>
       <c r="J136" t="inlineStr">
@@ -27910,7 +27910,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>Erin Maxwell</t>
+          <t>User 14405</t>
         </is>
       </c>
       <c r="J137" t="inlineStr">
@@ -28105,7 +28105,7 @@
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J138" t="inlineStr">
@@ -28313,7 +28313,7 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>Jo Stine</t>
+          <t>User 14406</t>
         </is>
       </c>
       <c r="J139" t="inlineStr">
@@ -28516,7 +28516,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>Amy Finley</t>
+          <t>User 14386</t>
         </is>
       </c>
       <c r="J140" t="inlineStr">
@@ -28722,7 +28722,7 @@
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>Patsy Bishop</t>
+          <t>User 14365</t>
         </is>
       </c>
       <c r="J141" t="inlineStr">
@@ -28925,7 +28925,7 @@
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>Patsy Bishop</t>
+          <t>User 14365</t>
         </is>
       </c>
       <c r="J142" t="inlineStr">
@@ -29128,7 +29128,7 @@
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>Theresa Mcgee</t>
+          <t>User 16178</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -29327,7 +29327,7 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>Caitlin Mellendorf</t>
+          <t>User 14548</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
@@ -29529,7 +29529,7 @@
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J145" t="inlineStr">
@@ -29742,7 +29742,7 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>Kristen Buttrum</t>
+          <t>User 14412</t>
         </is>
       </c>
       <c r="J146" t="inlineStr">
@@ -29942,7 +29942,7 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>Joey Fonseca</t>
+          <t>User 20553</t>
         </is>
       </c>
       <c r="J147" t="inlineStr">
@@ -30163,7 +30163,7 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>Nick Brown</t>
+          <t>User 20907</t>
         </is>
       </c>
       <c r="J148" t="inlineStr">
@@ -30363,7 +30363,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>Nick Brown</t>
+          <t>User 20907</t>
         </is>
       </c>
       <c r="J149" t="inlineStr">
@@ -30557,7 +30557,7 @@
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>Brenda E. Derrick</t>
+          <t>User 14570</t>
         </is>
       </c>
       <c r="J150" t="inlineStr">
@@ -30751,7 +30751,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>Sarita Sawyer</t>
+          <t>User 14363</t>
         </is>
       </c>
       <c r="J151" t="inlineStr">
@@ -30964,7 +30964,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>Erin Maxwell</t>
+          <t>User 14405</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
@@ -31119,7 +31119,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
@@ -31274,7 +31274,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J154" t="inlineStr">
@@ -31429,7 +31429,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>Della Jacobs</t>
+          <t>User 14782</t>
         </is>
       </c>
       <c r="J155" t="inlineStr">
@@ -31628,7 +31628,7 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>Della Jacobs</t>
+          <t>User 14782</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
@@ -31828,7 +31828,7 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>Della Jacobs</t>
+          <t>User 14782</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
@@ -32028,7 +32028,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>Della Jacobs</t>
+          <t>User 14782</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
@@ -32233,7 +32233,7 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>Della Jacobs</t>
+          <t>User 14782</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
@@ -32433,7 +32433,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>Patsy Bishop</t>
+          <t>User 14365</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
@@ -32637,7 +32637,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>Kaytlin Beekman</t>
+          <t>User 21859</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
@@ -32832,7 +32832,7 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
@@ -32988,7 +32988,7 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
@@ -33144,7 +33144,7 @@
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>Ashley Gilmour</t>
+          <t>User 19014</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
@@ -33343,7 +33343,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>Ashley Gilmour</t>
+          <t>User 19014</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
@@ -33548,7 +33548,7 @@
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J166" t="inlineStr">
@@ -33737,7 +33737,7 @@
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J167" t="inlineStr">
@@ -33926,7 +33926,7 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
@@ -34081,7 +34081,7 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>Michelle Fombelle</t>
+          <t>User 14565</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
@@ -34297,7 +34297,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>Michelle Fombelle</t>
+          <t>User 14565</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
@@ -34505,7 +34505,7 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
@@ -34660,7 +34660,7 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>Ana Lemke</t>
+          <t>User 14409</t>
         </is>
       </c>
       <c r="J172" t="inlineStr">
@@ -34860,7 +34860,7 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>Ashley Gilmour</t>
+          <t>User 19014</t>
         </is>
       </c>
       <c r="J173" t="inlineStr">
@@ -35059,7 +35059,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
@@ -35270,7 +35270,7 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>Rachel Benn</t>
+          <t>User 15793</t>
         </is>
       </c>
       <c r="J175" t="inlineStr">
@@ -35454,7 +35454,7 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>Pam Schallhorn</t>
+          <t>User 14290</t>
         </is>
       </c>
       <c r="J176" t="inlineStr">
@@ -35674,7 +35674,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>Pam Schallhorn</t>
+          <t>User 14290</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
@@ -35884,7 +35884,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
@@ -36098,7 +36098,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
@@ -36258,7 +36258,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
@@ -36413,7 +36413,7 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>Annette Reese</t>
+          <t>User 17883</t>
         </is>
       </c>
       <c r="J181" t="inlineStr">
@@ -36611,7 +36611,7 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>Pam Schallhorn</t>
+          <t>User 14290</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
@@ -36823,7 +36823,7 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>Darcy Eggimann</t>
+          <t>User 14435</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
@@ -37023,7 +37023,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>Brooke Desper</t>
+          <t>User 21080</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
@@ -37219,7 +37219,7 @@
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>Tracy Bowden</t>
+          <t>User 14356</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
@@ -37423,7 +37423,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>Nick Brown</t>
+          <t>User 20907</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
@@ -37623,7 +37623,7 @@
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J187" t="inlineStr">
@@ -37778,7 +37778,7 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>Natalie Coy</t>
+          <t>User 14401</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
@@ -37934,7 +37934,7 @@
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>Camaya Wallace Bechard</t>
+          <t>User 16465</t>
         </is>
       </c>
       <c r="J189" t="inlineStr">
@@ -38091,7 +38091,7 @@
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>Gina Adams</t>
+          <t>User 14578</t>
         </is>
       </c>
       <c r="J190" t="inlineStr">
@@ -38302,7 +38302,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>Julie Dantone</t>
+          <t>User 18475</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -38491,7 +38491,7 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>Patsy Bishop</t>
+          <t>User 14365</t>
         </is>
       </c>
       <c r="J192" t="inlineStr">
@@ -38694,7 +38694,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>Janette Saglier</t>
+          <t>User 16809</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
@@ -38849,7 +38849,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>Patsy Bishop</t>
+          <t>User 14365</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
@@ -39054,7 +39054,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>Barbara Curry</t>
+          <t>User 14366</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
@@ -39263,7 +39263,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>Ana Lemke</t>
+          <t>User 14409</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
@@ -39457,7 +39457,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>JoElyn Smith</t>
+          <t>User 14778</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
@@ -39646,7 +39646,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>Marcia Cruse</t>
+          <t>User 15185</t>
         </is>
       </c>
       <c r="J198" t="inlineStr">
@@ -39847,7 +39847,7 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>Julie Tyberendt Fulton</t>
+          <t>User 14408</t>
         </is>
       </c>
       <c r="J199" t="inlineStr">
@@ -40041,7 +40041,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>Julie Tyberendt Fulton</t>
+          <t>User 14408</t>
         </is>
       </c>
       <c r="J200" t="inlineStr">
@@ -40231,7 +40231,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>Jane Jones</t>
+          <t>User 22230</t>
         </is>
       </c>
       <c r="J201" t="inlineStr">
@@ -40436,7 +40436,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>Caitlin Kownacki</t>
+          <t>User 14562</t>
         </is>
       </c>
       <c r="J202" t="inlineStr">
@@ -40593,7 +40593,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>Caitlin Kownacki</t>
+          <t>User 14562</t>
         </is>
       </c>
       <c r="J203" t="inlineStr">
@@ -40750,7 +40750,7 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>Rebecca Crumrine</t>
+          <t>User 16163</t>
         </is>
       </c>
       <c r="J204" t="inlineStr">
@@ -40932,7 +40932,7 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>Rebecca Crumrine</t>
+          <t>User 16163</t>
         </is>
       </c>
       <c r="J205" t="inlineStr">
@@ -41105,7 +41105,7 @@
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J206" t="inlineStr">
@@ -41316,7 +41316,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>Melinda Vortman</t>
+          <t>User 14391</t>
         </is>
       </c>
       <c r="J207" t="inlineStr">
@@ -41525,7 +41525,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>Lacey Barnhill</t>
+          <t>User 14723</t>
         </is>
       </c>
       <c r="J208" t="inlineStr">
@@ -41703,7 +41703,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>Ana Lemke</t>
+          <t>User 14409</t>
         </is>
       </c>
       <c r="J209" t="inlineStr">
@@ -41863,7 +41863,7 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>Jenna Smith</t>
+          <t>User 14547</t>
         </is>
       </c>
       <c r="J210" t="inlineStr">
@@ -42076,7 +42076,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>Joey Fonseca</t>
+          <t>User 20553</t>
         </is>
       </c>
       <c r="J211" t="inlineStr">
@@ -42276,7 +42276,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>Rima Abusaid</t>
+          <t>User 16603</t>
         </is>
       </c>
       <c r="J212" t="inlineStr">
@@ -42489,7 +42489,7 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>Rima Abusaid</t>
+          <t>User 16603</t>
         </is>
       </c>
       <c r="J213" t="inlineStr">
@@ -42664,7 +42664,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>Dale Kehr</t>
+          <t>User 14566</t>
         </is>
       </c>
       <c r="J214" t="inlineStr">
@@ -42874,7 +42874,7 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>Misty Bernhard</t>
+          <t>User 20909</t>
         </is>
       </c>
       <c r="J215" t="inlineStr">
@@ -43074,7 +43074,7 @@
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>Cindy Glavin</t>
+          <t>User 18943</t>
         </is>
       </c>
       <c r="J216" t="inlineStr">
@@ -43277,7 +43277,7 @@
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t>Cindy Glavin</t>
+          <t>User 18943</t>
         </is>
       </c>
       <c r="J217" t="inlineStr">
@@ -43482,7 +43482,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>Cindy Glavin</t>
+          <t>User 18943</t>
         </is>
       </c>
       <c r="J218" t="inlineStr">
@@ -43688,7 +43688,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>Cindy Glavin</t>
+          <t>User 18943</t>
         </is>
       </c>
       <c r="J219" t="inlineStr">
@@ -43855,6 +43855,1352 @@
       </c>
       <c r="BE219" s="7" t="n">
         <v>44727.67510416666</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>26438</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Blessing Box for Lovington</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>0</v>
+      </c>
+      <c r="D220" t="n">
+        <v>1</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>University of Illinois Extension</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>User 14400</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>14400@fake_domain.com</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>User 14400</t>
+        </is>
+      </c>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>User 14399, User 14400, User 21464</t>
+        </is>
+      </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>SNAP-Ed</t>
+        </is>
+      </c>
+      <c r="L220" t="n">
+        <v>25315</v>
+      </c>
+      <c r="M220" t="inlineStr">
+        <is>
+          <t>Lovington Christian Church</t>
+        </is>
+      </c>
+      <c r="N220" t="n">
+        <v>0</v>
+      </c>
+      <c r="O220" t="inlineStr">
+        <is>
+          <t>Faith-based centers/places of worship</t>
+        </is>
+      </c>
+      <c r="P220" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="Q220" t="inlineStr">
+        <is>
+          <t>301 S County</t>
+        </is>
+      </c>
+      <c r="R220" t="inlineStr">
+        <is>
+          <t>Lovington</t>
+        </is>
+      </c>
+      <c r="S220" t="inlineStr">
+        <is>
+          <t>Moultrie</t>
+        </is>
+      </c>
+      <c r="T220" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="U220" t="n">
+        <v>61937</v>
+      </c>
+      <c r="V220" t="inlineStr"/>
+      <c r="W220" t="inlineStr">
+        <is>
+          <t>Moultrie (County)</t>
+        </is>
+      </c>
+      <c r="X220" t="inlineStr"/>
+      <c r="Y220" t="inlineStr"/>
+      <c r="Z220" t="n">
+        <v>18447</v>
+      </c>
+      <c r="AA220" t="inlineStr">
+        <is>
+          <t>Health: Chronic Disease Prevention and Management (State - 2021-2022)</t>
+        </is>
+      </c>
+      <c r="AB220" t="n">
+        <v>18447</v>
+      </c>
+      <c r="AC220" t="inlineStr">
+        <is>
+          <t>Health: Chronic Disease Prevention and Management (State - 2021-2022)</t>
+        </is>
+      </c>
+      <c r="AD220" t="inlineStr"/>
+      <c r="AE220" t="inlineStr">
+        <is>
+          <t>see attached file</t>
+        </is>
+      </c>
+      <c r="AF220" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH220" t="inlineStr"/>
+      <c r="AI220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lovington Illinois is a rural village in Moultrie County without an existing grocery store and a minimum 20 mile round trip to purchase groceries. They have a very active food pantry (Christ's Pantry) provided by the Lovington Christian Church. The pantry is open two afternoons per month. Their school is also over 70% free and reduced lunch eligible. Lovington is also home to many senior citizens on a fixed income.
+Because Lovington residents needed an extra boost to reduce their food insecurity issues, the idea of a blessing box was created.
+Funds to build the blessing box were provided through some surplus dollars from an Illinois Innovation Grant through Eastern Illinois University and the box was built by an Amish business specializing in recycled plastic building material.
+A committee of Lovington concern citizens (Hometown Love) agreed to finance the frame and concrete to support the box. Hometown Love also plans to landscape the area and add baskets at the bottom of the box.
+With the permission of the Lovington Village Board, the box was placed on the Lovington Community Garden site and next to the Lovington Police Department.
+Christ's Pantry volunteers have agreed to monitor the box and stock the shelves when necessary. SNAP-Ed staff will provide fresh produce during the growing season through the Partners In Produce program. 
+At this writing, the box has been in place for one week and it has been reported that not only is the community utilizing the box as well as leaving donations for others.
+</t>
+        </is>
+      </c>
+      <c r="AJ220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">see above
+</t>
+        </is>
+      </c>
+      <c r="AK220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"This is so awesome!"  Jane Franklin, Christ's Pantry Food Pantry Manager
+</t>
+        </is>
+      </c>
+      <c r="AL220" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO220" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT220" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU220" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ220" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA220" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB220" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC220" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD220" s="7" t="n">
+        <v>44735.47848379629</v>
+      </c>
+      <c r="BE220" s="7" t="n">
+        <v>44736.56869212963</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>26441</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Illinois Jr. Chef-Roasted Potatoes</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>0</v>
+      </c>
+      <c r="D221" t="n">
+        <v>1</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>University of Illinois Extension</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>User 14412</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>14412@fake_domain.com</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>User 14412</t>
+        </is>
+      </c>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>User 14412</t>
+        </is>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>SNAP-Ed</t>
+        </is>
+      </c>
+      <c r="L221" t="n">
+        <v>25413</v>
+      </c>
+      <c r="M221" t="inlineStr">
+        <is>
+          <t>Summersville Baptist Church</t>
+        </is>
+      </c>
+      <c r="N221" t="n">
+        <v>0</v>
+      </c>
+      <c r="O221" t="inlineStr">
+        <is>
+          <t>Faith-based centers/places of worship</t>
+        </is>
+      </c>
+      <c r="P221" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="Q221" t="inlineStr">
+        <is>
+          <t>1114 Fairfield Rd</t>
+        </is>
+      </c>
+      <c r="R221" t="inlineStr">
+        <is>
+          <t>Mount Vernon</t>
+        </is>
+      </c>
+      <c r="S221" t="inlineStr">
+        <is>
+          <t>Jefferson</t>
+        </is>
+      </c>
+      <c r="T221" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="U221" t="n">
+        <v>62864</v>
+      </c>
+      <c r="V221" t="inlineStr"/>
+      <c r="W221" t="inlineStr">
+        <is>
+          <t>Jefferson (County)</t>
+        </is>
+      </c>
+      <c r="X221" t="inlineStr"/>
+      <c r="Y221" t="inlineStr"/>
+      <c r="Z221" t="inlineStr"/>
+      <c r="AA221" t="inlineStr"/>
+      <c r="AB221" t="inlineStr"/>
+      <c r="AC221" t="inlineStr"/>
+      <c r="AD221" t="inlineStr"/>
+      <c r="AE221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Illinois Jr. Chef Program at Summersville Bapt. Church
+</t>
+        </is>
+      </c>
+      <c r="AF221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH221" t="inlineStr"/>
+      <c r="AI221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Illinois Junior Chef
+</t>
+        </is>
+      </c>
+      <c r="AJ221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An Illinois Junior Chef participant came back to cooking school the day after we had made Roasted Potatoes. She was so excited to tell, " I made the potato recipe last night at home for my family. It turned out really good and my family loved it. I did it all by myself, without any help." Illinois Junior Chef program helps our young participants be more independent and able to make healthier choices. 
+</t>
+        </is>
+      </c>
+      <c r="AK221" t="inlineStr"/>
+      <c r="AL221" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO221" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS221" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX221" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY221" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ221" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA221" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB221" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC221" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD221" s="7" t="n">
+        <v>44735.59443287037</v>
+      </c>
+      <c r="BE221" s="7" t="n">
+        <v>44735.60046296296</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>26449</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Annual Strong Families Community Resource Fair</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>0</v>
+      </c>
+      <c r="D222" t="n">
+        <v>1</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>University of Illinois Extension</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>User 14409</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>14409@fake_domain.com</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>User 14409</t>
+        </is>
+      </c>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>User 14409</t>
+        </is>
+      </c>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>SNAP-Ed</t>
+        </is>
+      </c>
+      <c r="L222" t="inlineStr"/>
+      <c r="M222" t="inlineStr"/>
+      <c r="N222" t="inlineStr"/>
+      <c r="O222" t="inlineStr"/>
+      <c r="P222" t="inlineStr"/>
+      <c r="Q222" t="inlineStr"/>
+      <c r="R222" t="inlineStr"/>
+      <c r="S222" t="inlineStr"/>
+      <c r="T222" t="inlineStr"/>
+      <c r="U222" t="inlineStr"/>
+      <c r="V222" t="inlineStr"/>
+      <c r="W222" t="inlineStr">
+        <is>
+          <t>St. Clair (County)</t>
+        </is>
+      </c>
+      <c r="X222" t="inlineStr"/>
+      <c r="Y222" t="inlineStr"/>
+      <c r="Z222" t="inlineStr"/>
+      <c r="AA222" t="inlineStr"/>
+      <c r="AB222" t="inlineStr"/>
+      <c r="AC222" t="inlineStr"/>
+      <c r="AD222" t="inlineStr"/>
+      <c r="AE222" t="inlineStr"/>
+      <c r="AF222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH222" t="inlineStr"/>
+      <c r="AI222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Community Resource Fair in E. St. Louis the target audience was for families  with children and senior too. 
+</t>
+        </is>
+      </c>
+      <c r="AJ222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was at the Resources Fair for families and some clients ask me how the popcorn was made I explained to them that It was ease to make it home Just limited your salt when you make it. they were so happy to hear hoe easy is to pop some popcorn and make it
+healthy for the family, she thank to me for the tips how to make it . she told me know i will ho home and pop and use this ingredients. She told me thank you for those easy healthy tips. 
+</t>
+        </is>
+      </c>
+      <c r="AK222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy that they going to make this healthy popcorn flavors
+</t>
+        </is>
+      </c>
+      <c r="AL222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM222" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO222" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS222" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX222" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY222" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ222" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA222" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB222" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC222" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD222" s="7" t="n">
+        <v>44736.45388888889</v>
+      </c>
+      <c r="BE222" s="7" t="n">
+        <v>44736.47002314815</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>26451</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Many Hands Make Light Work</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>0</v>
+      </c>
+      <c r="D223" t="n">
+        <v>1</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>University of Illinois Extension</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>User 14400</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>14400@fake_domain.com</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>User 14400</t>
+        </is>
+      </c>
+      <c r="J223" t="inlineStr">
+        <is>
+          <t>User 14399, User 14400, User 21464</t>
+        </is>
+      </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>SNAP-Ed</t>
+        </is>
+      </c>
+      <c r="L223" t="n">
+        <v>132503</v>
+      </c>
+      <c r="M223" t="inlineStr">
+        <is>
+          <t>Sullivan United Methodist Church</t>
+        </is>
+      </c>
+      <c r="N223" t="n">
+        <v>0</v>
+      </c>
+      <c r="O223" t="inlineStr">
+        <is>
+          <t>Faith-based centers/places of worship</t>
+        </is>
+      </c>
+      <c r="P223" t="inlineStr">
+        <is>
+          <t>live</t>
+        </is>
+      </c>
+      <c r="Q223" t="inlineStr">
+        <is>
+          <t>216 W. Jefferson Street</t>
+        </is>
+      </c>
+      <c r="R223" t="inlineStr">
+        <is>
+          <t>Sullivan</t>
+        </is>
+      </c>
+      <c r="S223" t="inlineStr">
+        <is>
+          <t>Moultrie</t>
+        </is>
+      </c>
+      <c r="T223" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="U223" t="n">
+        <v>61951</v>
+      </c>
+      <c r="V223" t="inlineStr"/>
+      <c r="W223" t="inlineStr">
+        <is>
+          <t>Moultrie (County)</t>
+        </is>
+      </c>
+      <c r="X223" t="inlineStr"/>
+      <c r="Y223" t="inlineStr"/>
+      <c r="Z223" t="n">
+        <v>18447</v>
+      </c>
+      <c r="AA223" t="inlineStr">
+        <is>
+          <t>Health: Chronic Disease Prevention and Management (State - 2021-2022)</t>
+        </is>
+      </c>
+      <c r="AB223" t="n">
+        <v>18447</v>
+      </c>
+      <c r="AC223" t="inlineStr">
+        <is>
+          <t>Health: Chronic Disease Prevention and Management (State - 2021-2022)</t>
+        </is>
+      </c>
+      <c r="AD223" t="inlineStr">
+        <is>
+          <t>Food Insecurity</t>
+        </is>
+      </c>
+      <c r="AE223" t="inlineStr"/>
+      <c r="AF223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH223" t="inlineStr"/>
+      <c r="AI223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decatur Catholic Charities have been a food mobile partner sine the beginning of the pandemic.
+</t>
+        </is>
+      </c>
+      <c r="AJ223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decatur Catholic Charities approached SNAP-Ed staff about the possibility of extending their reach into the Sullivan area for possible food mobile dates. PSE staff contacted Sullivan United Methodist Church and connected them with Catholic Charities and set the first food distribution date for June 22, 2022. PSE staff worked with the church and Catholic Charities to get participants registered. The final registration total was 149 families.
+On the day of distribution, SNAP-Ed staff assisted church volunteers with sorting, packing, delivering and distribution. Snap staff also provided fresh produce from the Arthur Produce Auction to each family and an Eat Move Save booth on site.
+Plans to continue the mobile pantries are in place and the next one scheduled is August 24, 2022.
+</t>
+        </is>
+      </c>
+      <c r="AK223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"While watching the activities around our pavilion I know I saw the hands and feet of Christ at work in our community." - Cheryl Thomas Sullivan United Methodist Church
+</t>
+        </is>
+      </c>
+      <c r="AL223" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO223" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS223" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT223" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ223" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA223" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB223" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC223" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD223" s="7" t="n">
+        <v>44736.57097222222</v>
+      </c>
+      <c r="BE223" s="7" t="n">
+        <v>44736.58762731482</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>26452</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Lettuce Go To The School Garden</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>0</v>
+      </c>
+      <c r="D224" t="n">
+        <v>1</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>University of Illinois Extension</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>16809@fake_domain.com</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="J224" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>SNAP-Ed</t>
+        </is>
+      </c>
+      <c r="L224" t="n">
+        <v>19913</v>
+      </c>
+      <c r="M224" t="inlineStr">
+        <is>
+          <t>Perry Elem School</t>
+        </is>
+      </c>
+      <c r="N224" t="n">
+        <v>0</v>
+      </c>
+      <c r="O224" t="inlineStr">
+        <is>
+          <t>Schools (K-12, elementary, middle, and high)</t>
+        </is>
+      </c>
+      <c r="P224" t="inlineStr">
+        <is>
+          <t>learn</t>
+        </is>
+      </c>
+      <c r="Q224" t="inlineStr">
+        <is>
+          <t>633 W Perry St</t>
+        </is>
+      </c>
+      <c r="R224" t="inlineStr">
+        <is>
+          <t>Belvidere</t>
+        </is>
+      </c>
+      <c r="S224" t="inlineStr">
+        <is>
+          <t>Boone</t>
+        </is>
+      </c>
+      <c r="T224" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="U224" t="n">
+        <v>61008</v>
+      </c>
+      <c r="V224" t="inlineStr"/>
+      <c r="W224" t="inlineStr">
+        <is>
+          <t>Boone (County)</t>
+        </is>
+      </c>
+      <c r="X224" t="inlineStr"/>
+      <c r="Y224" t="inlineStr"/>
+      <c r="Z224" t="inlineStr"/>
+      <c r="AA224" t="inlineStr"/>
+      <c r="AB224" t="inlineStr"/>
+      <c r="AC224" t="inlineStr"/>
+      <c r="AD224" t="inlineStr"/>
+      <c r="AE224" t="inlineStr"/>
+      <c r="AF224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH224" t="inlineStr"/>
+      <c r="AI224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This story is about a boy who was part of The Great Garden Detective program during his third grade year (2021-2022) at Perry Elementary School, 622 West Perry Street, Belvidere. He has also enrolled in the CATCH summer program, which started two weeks after school ended and is held at the Perry School Garden that he helped to plant.
+</t>
+        </is>
+      </c>
+      <c r="AJ224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">During the spring Perry Elementary School third and fourth graders were part of The Great Garden Detective Adventure program and they planted a school garden. Two weeks after the school year ended, we started a CATCH program in conjunction with a Master Gardener. We are going to learn about fruits and vegetables, and get some physical exercise followed by the students keeping up the garden with the Master Gardener's assistance. The first day of CATCH, one of the soon to be fourth graders, told me how he, his brother and mother live a few houses down from the school and came to the garden and picked some lettuce. The student said his mother put some of the garden fresh lettuce on his sandwich, which he has never tried before, and he liked. Now he puts lettuce on most of his sandwiches. The Master Gardener said that he would put in a fall crop of lettuce so they can have as much as they would like. When you plant and care for a garden you are more inclined to try foods you are unfamiliar with.
+</t>
+        </is>
+      </c>
+      <c r="AK224" t="inlineStr"/>
+      <c r="AL224" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN224" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO224" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS224" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX224" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ224" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA224" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB224" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC224" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD224" s="7" t="n">
+        <v>44736.6275</v>
+      </c>
+      <c r="BE224" s="7" t="n">
+        <v>44736.64336805556</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>26453</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Helpful Lesson</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>0</v>
+      </c>
+      <c r="D225" t="n">
+        <v>1</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>University of Illinois Extension</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>16809@fake_domain.com</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="J225" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>SNAP-Ed</t>
+        </is>
+      </c>
+      <c r="L225" t="inlineStr"/>
+      <c r="M225" t="inlineStr"/>
+      <c r="N225" t="inlineStr"/>
+      <c r="O225" t="inlineStr"/>
+      <c r="P225" t="inlineStr"/>
+      <c r="Q225" t="inlineStr"/>
+      <c r="R225" t="inlineStr"/>
+      <c r="S225" t="inlineStr"/>
+      <c r="T225" t="inlineStr"/>
+      <c r="U225" t="inlineStr"/>
+      <c r="V225" t="inlineStr"/>
+      <c r="W225" t="inlineStr">
+        <is>
+          <t>Boone (County)</t>
+        </is>
+      </c>
+      <c r="X225" t="inlineStr"/>
+      <c r="Y225" t="inlineStr"/>
+      <c r="Z225" t="inlineStr"/>
+      <c r="AA225" t="inlineStr"/>
+      <c r="AB225" t="inlineStr"/>
+      <c r="AC225" t="inlineStr"/>
+      <c r="AD225" t="inlineStr"/>
+      <c r="AE225" t="inlineStr"/>
+      <c r="AF225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH225" t="inlineStr"/>
+      <c r="AI225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was doing and Eat Move Save Booth at Empower Boone pantry, 200 South Fifth Street, Capron, and crossed paths with an individual who had attended my Healthy Cents class, during a WIC clinic at the Boone County Health Department, 1204 Logan Avenue, Belvidere.
+</t>
+        </is>
+      </c>
+      <c r="AJ225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was doing and Eat Move Save Booth at a pantry when I crossed paths with an individual who had attended my Healthy Cents class. She stated that it was the lesson on snacks that she attended. She said that she made the trail mix, because she had all of the ingredients on hand, and her children and their friends really liked it. She also told me that she looked at the cracker box she had to find out the number of servings and the portion size. She filled baggies each with one portion of the crackers. She thanked me for the idea, stating snacks are so expensive, especially when the kids are home on summer break. Proper portion size of foods prevents over eating, weight gain and saves money.
+</t>
+        </is>
+      </c>
+      <c r="AK225" t="inlineStr"/>
+      <c r="AL225" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO225" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS225" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX225" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ225" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA225" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB225" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC225" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD225" s="7" t="n">
+        <v>44736.64435185185</v>
+      </c>
+      <c r="BE225" s="7" t="n">
+        <v>44736.65769675926</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>26465</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Lavender farm tour</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>1</v>
+      </c>
+      <c r="D226" t="n">
+        <v>0</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>University of Illinois Extension</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>User 14703</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>14703@fake_domain.com</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>User 14703</t>
+        </is>
+      </c>
+      <c r="J226" t="inlineStr">
+        <is>
+          <t>User 14703</t>
+        </is>
+      </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>Agriculture and Agribusiness</t>
+        </is>
+      </c>
+      <c r="L226" t="n">
+        <v>36184</v>
+      </c>
+      <c r="M226" t="inlineStr">
+        <is>
+          <t>U of I Extension - Jefferson Co - Mt Vernon</t>
+        </is>
+      </c>
+      <c r="N226" t="n">
+        <v>0</v>
+      </c>
+      <c r="O226" t="inlineStr">
+        <is>
+          <t>Extension offices</t>
+        </is>
+      </c>
+      <c r="P226" t="inlineStr">
+        <is>
+          <t>learn</t>
+        </is>
+      </c>
+      <c r="Q226" t="inlineStr">
+        <is>
+          <t>4618 Broadway</t>
+        </is>
+      </c>
+      <c r="R226" t="inlineStr">
+        <is>
+          <t>Mount Vernon</t>
+        </is>
+      </c>
+      <c r="S226" t="inlineStr">
+        <is>
+          <t>Jefferson</t>
+        </is>
+      </c>
+      <c r="T226" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="U226" t="n">
+        <v>62864</v>
+      </c>
+      <c r="V226" t="inlineStr"/>
+      <c r="W226" t="inlineStr">
+        <is>
+          <t>Jefferson (County)</t>
+        </is>
+      </c>
+      <c r="X226" t="n">
+        <v>415873</v>
+      </c>
+      <c r="Y226" t="inlineStr">
+        <is>
+          <t>Growing Lavender in Southern Illinois</t>
+        </is>
+      </c>
+      <c r="Z226" t="n">
+        <v>18445</v>
+      </c>
+      <c r="AA226" t="inlineStr">
+        <is>
+          <t>Environment: Engagement with Home and Community Landscapes and Environment (State - 2021-2022)</t>
+        </is>
+      </c>
+      <c r="AB226" t="n">
+        <v>18445</v>
+      </c>
+      <c r="AC226" t="inlineStr">
+        <is>
+          <t>Environment: Engagement with Home and Community Landscapes and Environment (State - 2021-2022)</t>
+        </is>
+      </c>
+      <c r="AD226" t="inlineStr">
+        <is>
+          <t>Gardening, Health</t>
+        </is>
+      </c>
+      <c r="AE226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of the participants that attended the Growing Lavender in Southern Illinois and went on the farm tour sent this message after the event. 
+Erin Berry " Visiting the lavender farm was not only a fun experience, but also educational. Learning the best way to plant, harvest, and grow lavender from cuttings will hopefully help me successfully grow some beautiful and fragrant lavender." 
+</t>
+        </is>
+      </c>
+      <c r="AF226" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG226" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH226" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI226" t="inlineStr"/>
+      <c r="AJ226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christina Lueking, Horticulture educator led a presentation on how to grow, plant and harvest locally grown lavender in Southern Illinois. 
+</t>
+        </is>
+      </c>
+      <c r="AK226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Erin Berry " Visiting the lavender farm was not only a fun experience, but also educational. Learning the best way to plant, harvest, and grow lavender from cuttings will hopefully help me successfully grow some beautiful and fragrant lavender."  
+</t>
+        </is>
+      </c>
+      <c r="AL226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY226" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ226" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA226" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB226" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC226" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD226" s="7" t="n">
+        <v>44739.58363425926</v>
+      </c>
+      <c r="BE226" s="7" t="n">
+        <v>44739.58472222222</v>
       </c>
     </row>
   </sheetData>
@@ -43868,7 +45214,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E337"/>
+  <dimension ref="A1:E348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50494,6 +51840,215 @@
       </c>
       <c r="E337" t="inlineStr"/>
     </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>26438</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>User 14399</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>0</v>
+      </c>
+      <c r="E338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>26438</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>User 14400</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>1</v>
+      </c>
+      <c r="E339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>26438</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>User 21464</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>0</v>
+      </c>
+      <c r="E340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>26441</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>User 14412</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>1</v>
+      </c>
+      <c r="E341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>26449</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>User 14409</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>1</v>
+      </c>
+      <c r="E342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>26451</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>User 14399</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>0</v>
+      </c>
+      <c r="E343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>26451</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>User 14400</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>1</v>
+      </c>
+      <c r="E344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>26451</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>User 21464</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>0</v>
+      </c>
+      <c r="E345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>26452</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>1</v>
+      </c>
+      <c r="E346" t="inlineStr"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>26453</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>User 16809</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>1</v>
+      </c>
+      <c r="E347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>26465</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>User 14703</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>edit</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>1</v>
+      </c>
+      <c r="E348" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>